<commit_message>
Fix(all scripts): Updating routes for __tmp__ files
</commit_message>
<xml_diff>
--- a/__src__/__tmp__/tmp_factores.xlsx
+++ b/__src__/__tmp__/tmp_factores.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24527"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Diego\Desktop\Koening\HuffModel\huff-model-macro\__src__\__tmp__\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A9C2445-A153-49C6-A209-231FCD91158F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C4D200B-EBDB-474B-89F9-43788097385E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>nombre</t>
   </si>
@@ -28,13 +28,25 @@
     <t>factor</t>
   </si>
   <si>
+    <t>Hipermercado Metro Independencia</t>
+  </si>
+  <si>
     <t>Plaza Vea Izaguirre</t>
   </si>
   <si>
+    <t>Tottus Mega Plaza</t>
+  </si>
+  <si>
     <t>Plaza Vea Los Olivos</t>
   </si>
   <si>
-    <t>Plaza Vea Universitaria</t>
+    <t>Tottus Los Olivos</t>
+  </si>
+  <si>
+    <t>Makro Plaza Lima Norte</t>
+  </si>
+  <si>
+    <t>Makro Comas</t>
   </si>
   <si>
     <t>Supermercado</t>
@@ -440,7 +452,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Hoja1"/>
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -456,7 +468,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="B2">
         <v>8</v>
@@ -467,7 +479,7 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -475,7 +487,7 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -483,7 +495,39 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <v>4</v>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>